<commit_message>
add reader function for excel files
</commit_message>
<xml_diff>
--- a/test-data/user-info/user-info.xlsx
+++ b/test-data/user-info/user-info.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>firstName</t>
   </si>
@@ -46,6 +46,42 @@
   </si>
   <si>
     <t>Abcd@1234</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>0912345678</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>no.password_playwright.ts@example.com</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>no.company_playwright.ts@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Row After</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>row.after.empty_playwright.ts@example.com</t>
+  </si>
+  <si>
+    <t>Formular</t>
+  </si>
+  <si>
+    <t>Row</t>
   </si>
 </sst>
 </file>
@@ -101,11 +137,13 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="1" applyFont="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="1" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -652,10 +690,91 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" ht="14.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="str">
+        <f>LOWER(A8)&amp;"."&amp;LOWER(B8)&amp;"_playwright.ts@example.com"</f>
+        <v>formular.row_playwright.ts@example.com</v>
+      </c>
+      <c r="E8">
+        <f>12345+54321</f>
+        <v>66666</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="D2"/>
     <hyperlink r:id="rId2" ref="E2"/>
+    <hyperlink r:id="rId3" ref="D4"/>
+    <hyperlink r:id="rId4" ref="D5"/>
+    <hyperlink r:id="rId5" ref="D7"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>